<commit_message>
Averaging over annotations. WORKS
Scrambling and seeing.
</commit_message>
<xml_diff>
--- a/clean/shalek.xlsx
+++ b/clean/shalek.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1875" uniqueCount="1875">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1876" uniqueCount="1876">
   <si>
     <t>On_Chip_Stimulation_LPS_4h_S10</t>
   </si>
@@ -5644,6 +5644,9 @@
   </si>
   <si>
     <t>MFNG</t>
+  </si>
+  <si>
+    <t>b</t>
   </si>
 </sst>
 </file>
@@ -6014,7 +6017,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BSP15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="BSF1" workbookViewId="0">
+      <selection activeCell="BSP2" sqref="BSP2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
@@ -11601,6 +11606,9 @@
       </c>
       <c r="BSO1" t="s">
         <v>1860</v>
+      </c>
+      <c r="BSP1" t="s">
+        <v>1875</v>
       </c>
     </row>
     <row r="2" spans="1:1862">

</xml_diff>